<commit_message>
feat : themes.xlsx 파일 업데이트
</commit_message>
<xml_diff>
--- a/src/main/resources/data/themes.xlsx
+++ b/src/main/resources/data/themes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaahyeonseo/Desktop/Spring/Bjjm/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F43EB57-BE4A-C447-9EE4-C948518C58D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BF91D9-2C74-7C42-A1E6-5DE65BD6C2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="23640" windowHeight="15680" xr2:uid="{7ABD076A-39D2-8341-A844-6079A1F4869C}"/>
+    <workbookView xWindow="1200" yWindow="760" windowWidth="28200" windowHeight="15680" xr2:uid="{7ABD076A-39D2-8341-A844-6079A1F4869C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="135">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1222,12 +1222,2272 @@
     <t>FAMILY_WITH_CHILD,LOCAL_TOUR,DATE_COURSE,CAFE_PHOTO,LOCAL_COURSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>☕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 파도 소리와 함께, 오션뷰 카페 순례</t>
+    </r>
+  </si>
+  <si>
+    <t>푸른 바다를 보며 즐기는 커피 한 잔의 여유. 부산이기에 가능한 최고의 힐링 코스입니다.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 카페 385
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 영도구 태종로 539
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 총총커피, 바스크 치즈 케이크
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>☕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 오션뷰 특징: 통유리창 너머로 부산 남항과 배들이 지나다니는 풍경을 감상할 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 해 질 녘 노을이 아름다운 곳으로, 창가 자리를 원한다면 일찍 방문하는 것을 추천합니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 영도구 태종로 539</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 웨이브온 커피
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 기장군 장안읍 해맞이로 286
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 월내 라떼, 풀문 커피
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>☕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 오션뷰 특징: 건축상을 받은 독특한 건물 디자인과 바로 앞까지 파도가 밀려오는 듯한 오션뷰가 특징입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 루프탑과 야외 평상 좌석 등 다양한 공간이 마련되어 있어 취향에 맞게 바다를 즐기기 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 기장군 장안읍 해맞이로 286</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CORALANI (코랄라니)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 기장군 기장읍 기장해안로 32
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 코랄라니 에이드, 베이커리류
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>☕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 오션뷰 특징: 해외 휴양지에 온 듯한 이국적인 인테리어와 야자수, 그리고 넓은 야외 정원에서 동해 바다를 만끽할 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 바로 옆 아난티 힐튼과 이어져 있어 함께 둘러보기 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 기장군 기장읍 기장해안로 32</t>
+  </si>
+  <si>
+    <t>DATE_COURSE</t>
+  </si>
+  <si>
+    <t>DATE_COURSE,CAFE_PHOTO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>🍜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 현지인 추천! 부산 대표 맛집 로드</t>
+    </r>
+  </si>
+  <si>
+    <t>관광객 맛집은 그만! 부산 토박이들이 사랑하는 찐 맛집에서 진짜 부산의 맛을 느껴보세요.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🐷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 쌍둥이돼지국밥
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 남구 유엔평화로 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🍴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 돼지국밥, 수육백반
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 현지인 꿀팁: 수육백반을 주문하면 국밥과 맛있는 수육을 함께 맛볼 수 있어 가성비가 좋습니다. 부추(정구지)를 듬뿍 넣어 드셔보세요.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 남구 유엔평화로 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🥟</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 신발원
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 동구 대영로243번길 62
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🍴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 고기만두, 군만두, 콩국+과자
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 현지인 꿀팁: 식사 시간대에는 대기가 매우 깁니다. 포장을 이용하거나, 비교적 한산한 평일 오전을 노리는 것이 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 동구 대영로243번길 62</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🐟</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 김유순대구뽈찜
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 남구 대연동 291-2 1층
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🍴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 대구뽈찜
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 현지인 꿀팁: 콩나물과 양념을 덜어 먹은 후 비벼 먹으세요 양념 추가와 사리추가는 필수</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 남구 대연동 291-2 1층</t>
+  </si>
+  <si>
+    <r>
+      <t>🌊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 바다를 통째로! 부산 해산물 맛집 정복</t>
+    </r>
+  </si>
+  <si>
+    <t>항구 도시 부산에 왔다면 신선한 해산물은 선택이 아닌 필수! 갓 잡은 해산물의 참맛을 제대로 느껴보세요.</t>
+  </si>
+  <si>
+    <t>ALLEY_TRIP,LOCAL_COURSE,SOLO_TRIP,FOOD_TOUR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOOD_TOUR,LOCAL_TOUR,LOCAL_COURSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🦞</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 자갈치시장
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 중구 자갈치해안로 52
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🍴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 제철 활어회, 꼼장어 구이, 해물 모듬
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 해산물 특징: 부산 최대의 수산물 시장. 1층에서 직접 횟감을 고른 뒤 2층 초장집에서 바로 맛볼 수 있는 시스템입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: '오이소, 보이소, 사이소'라는 정겨운 구호처럼 활기찬 시장 분위기를 느껴보세요. 가격 흥정은 필수!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 중구 자갈치해안로 52</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🦀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 미포끝집
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 해운대구 달맞이길62번길 77
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🍴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 조개구이, 장어구이
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 해산물 특징: 해운대 미포 선착장 끝에 위치하여 바다를 보며 조개구이와 장어구이를 즐길 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 해가 질 무렵 창가 자리에 앉으면 환상적인 노을과 야경을 배경으로 식사할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 해운대구 달맞이길62번길 77</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🐚</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 청사포 수민이네
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 해운대구 청사포로58번길 118
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🍴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 추천 메뉴: 조개구이, 장어구이
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 해산물 특징: 청사포 조개구이의 원조 격인 곳으로, 신선한 조개와 장어를 맛볼 수 있는 노포 맛집입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 조개를 다 먹은 뒤 남은 양념에 볶아 먹는 볶음밥이 별미입니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 해운대구 청사포로58번길 118</t>
+  </si>
+  <si>
+    <r>
+      <t>🛍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 전통과 현대의 조화, 쇼핑의 모든 것</t>
+    </r>
+  </si>
+  <si>
+    <t>활기 넘치는 전통시장부터 세련된 백화점까지, 부산에서 즐길 수 있는 다채로운 쇼핑의 세계로 안내합니다.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 국제시장 &amp; 부평깡통시장
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 중구 신창동4가
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 없는 것 빼고 다 있다는 만물 시장. 구제 옷, 수입 과자, 주방용품 등 구경하는 재미가 쏠쏠하며, 깡통시장의 야시장은 필수 코스입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 씨앗호떡, 비빔당면, 유부주머니 등 시장의 명물 먹거리들을 맛보며 쇼핑을 즐겨보세요.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 중구 신창동4가</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 신세계백화점 센텀시티점
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 해운대구 센텀남대로 35
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 세계 최대 규모로 기네스북에 등재된 백화점. 쇼핑은 물론 스파랜드, 아이스링크 등 다양한 엔터테인먼트 시설을 갖추고 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 쇼핑 후 '스파랜드'에서 온천욕을 즐기며 여행의 피로를 푸는 코스를 추천합니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 해운대구 센텀남대로 35</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 롯데프리미엄아울렛 동부산점
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 기장군 기장읍 기장해안로 147
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 그리스 산토리니를 모티브로 한 이국적인 건축물에서 다양한 브랜드를 합리적인 가격에 쇼핑할 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 아이들을 위한 놀이시설과 등대 전망대가 있어 가족 단위 쇼핑객에게 특히 인기가 많습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 기장군 기장읍 기장해안로 147</t>
+  </si>
+  <si>
+    <t>LOCAL_TOUR,DATE_COURSE,FAMILY_WITH_CHILD,SOLO_TRIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>🚶‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 몸과 마음의 힐링, 부산 걷기 좋은 길</t>
+    </r>
+  </si>
+  <si>
+    <t>복잡한 도심을 벗어나 부산의 아름다운 자연을 만끽하며 여유롭게 걸어보세요.</t>
+  </si>
+  <si>
+    <t>SOLO_TRIP,LOCAL_TOUR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 이기대 해안산책로
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 남구 용호동
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 바다 위를 걷는 듯한 오륙도 스카이워크에서 시작하여 해안 절경을 따라 걷는 길. 광안대교와 해운대 마천루를 조망할 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 전 구간(약 4.7km)을 걷기 부담스럽다면, 스카이워크 주변이나 동생말 부근만 가볍게 산책하는 것도 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 남구 용호동</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 태종대 유원지 (다누비 열차)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 영도구 전망로 24
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 울창한 숲과 깎아지른 듯한 기암괴석, 푸른 바다가 어우러진 부산의 대표적인 명승지입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: '다누비 열차'를 이용하면 주요 명소(전망대, 영도등대)를 편하게 둘러볼 수 있습니다. 날씨가 좋은 날에는 전망대에서 일본 대마도까지 보입니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 영도구 전망로 24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 해운대 동백섬
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 해운대구 우동
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 해운대 해수욕장 옆에 위치해 접근성이 좋으며, 동백나무와 소나무가 울창한 산책로가 조성되어 있습니다. 누리마루 APEC 하우스도 함께 볼 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 섬을 한 바퀴 도는 데 약 30~40분 정도 소요되어 아침이나 저녁 식사 후 가볍게 산책하기에 완벽한 코스입니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 해운대구 우동</t>
+  </si>
+  <si>
+    <r>
+      <t>💖</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 특별한 하루, 로맨틱 데이트 코스</t>
+    </r>
+  </si>
+  <si>
+    <t>연인과 함께라면 더욱 좋은, 아름다운 풍경과 특별한 경험이 가득한 로맨틱 스팟을 소개합니다.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💞</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 해운대 블루라인파크 (해변열차 &amp; 스카이캡슐)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 해운대구 청사포로 116
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 동해남부선 옛 철길을 따라 해운대 미포-청사포-송정의 아름다운 해안 절경을 감상할 수 있는 관광 열차입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 프라이빗한 스카이캡슐은 인기가 많아 온라인 사전 예매가 필수입니다. 미포 정거장에서 청사포 방향으로 탑승하는 코스의 뷰가 더 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 해운대구 청사포로 116</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💞</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 광안리 M 드론 라이트쇼
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 수영구 광안해변로 219
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 매주 토요일 저녁, 광안대교를 배경으로 수백 대의 드론이 펼치는 환상적인 라이트 쇼가 펼쳐집니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 계절과 행사에 따라 공연 시간과 횟수가 변경될 수 있으니 방문 전 '수영구청' 홈페이지를 꼭 확인하세요.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 수영구 광안해변로 219</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💞</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 송도 해상케이블카
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 서구 송도해변로 171
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 송도해수욕장 동쪽 송림공원에서 서쪽 암남공원까지 바다 위를 가로지르며 부산의 해안 풍경을 즐길 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 바닥이 투명한 '크리스탈 크루즈'를 탑승하면 발밑으로 푸른 바다가 펼쳐져 더욱 스릴 있는 경험을 할 수 있습니다.3</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 서구 송도해변로 171</t>
+  </si>
+  <si>
+    <r>
+      <t>♨️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 여기 부산 맞아? 이색 체험 스팟</t>
+    </r>
+  </si>
+  <si>
+    <t>맛집과 관광지를 넘어, 오직 부산에서만 즐길 수 있는 특별하고 색다른 체험으로 여행의 재미를 더해보세요.</t>
+  </si>
+  <si>
+    <t>FAMILY_WITH_CHILD,LOCAL_TOUR,SOLO_TRIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🧗‍♀️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 웨이브락
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산광역시 금정구 장전온</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic Semilight"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>﻿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">천천로 51
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 호텔 농심 건물에 위치한 대규모 실내 액티비티 시설. 클라이밍, 트램펄린 등 다양한 스포츠를 안전하게 즐길 수 있습니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 바로 옆에 부산대 카페거리가 있어, 신나게 액티비티를 즐긴 후 분위기 좋은 카페가면 완벽한 코스가 됩니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산광역시 금정구 장전온﻿천천로 51</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🏞️</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 아홉산숲
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 기장군 철마면 미동길 37-1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 400년 동안 가꿔온 사유림으로, 영화 '군도', '대호', 드라마 '더 킹: 영원의 군주' 등의 촬영지. 잘 보존된 대나무 숲이 장관입니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 숲 보호를 위해 제한된 인원만 입장 가능하므로, 방문 전 운영 시간을 확인하는 것이 좋습니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 기장군 철마면 미동길 37-1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🛕</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 삼광사
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>📍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 위치: 부산 부산진구 초읍천로43번길 77
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 주요 특징: 도심 속에 위치한 거대한 규모의 사찰로, 특히 부처님 오신 날이 되면 수만 개의 연등이 불을 밝혀 장관을 이룹니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>💡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 팁: 연등 축제 기간이 아니더라도 고즈넉한 사찰을 산책하며 마음의 평화를 찾기 좋은 곳입니다. 다채로운 색의 연등 터널은 언제나 아름다운 포토존입니다.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 부산진구 초읍천로43번길 77</t>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/4_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/4_img1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/4_img3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/5_img1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/5_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/5_ing3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/6_ing1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/6_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/6_img3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/7_img1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/7_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/7_img3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/8_img1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/8_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/8_img3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/9_img1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/9_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/9_img3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/10_img1.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/10_img2.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://bjjm-bucket.s3.ap-northeast-2.amazonaws.com/themes/10_img3.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1274,6 +3534,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Apple Color Emoji"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic Semilight"/>
       <family val="2"/>
       <charset val="129"/>
     </font>
@@ -1654,9 +3921,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11B0491-5473-C74B-9E12-12DEC8DB487B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1930,6 +4197,426 @@
         <v>46</v>
       </c>
     </row>
+    <row r="14" spans="1:6" ht="163">
+      <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="163">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="144">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="119">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="119">
+      <c r="A18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="119">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="163">
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="163">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="163">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="157">
+      <c r="A23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="157">
+      <c r="A24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="138">
+      <c r="A25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="157">
+      <c r="A26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="157">
+      <c r="A27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="157">
+      <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="176">
+      <c r="A29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="138">
+      <c r="A30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="138">
+      <c r="A31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="138">
+      <c r="A32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="157">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="157">
+      <c r="A34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1945,6 +4632,27 @@
     <hyperlink ref="F12" r:id="rId10" xr:uid="{5BACB917-2F16-D14D-A7D9-01358E7FD619}"/>
     <hyperlink ref="F13" r:id="rId11" xr:uid="{51EEDA54-7E84-AE48-8D9A-C79284FC45D0}"/>
     <hyperlink ref="F3" r:id="rId12" xr:uid="{60BBCA33-B71B-7A44-B671-D0D633D5CAFD}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{070A0B40-9BF1-2849-97A6-C04CE35FCB0F}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{21733B82-8D5A-E941-83FE-ADDB56760EAA}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{FA0883AD-A2D6-EF49-A9AD-567C2A916F2F}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{3C69AECD-C238-A349-987C-BE14DDE697B7}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{06A097CF-DED4-0942-9AC6-5FBA12B5377E}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{13AF6F51-EEDD-3A4F-82DB-089EDCB9A300}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{FFB1D318-DE39-4A46-9923-C9965C844852}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{7D9D6CE5-2D6F-A940-A888-CD92E3E4ECD5}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{B6F77562-6CBF-584F-9AA3-504FE24BCC5F}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{B3A5BA31-1B01-1F4A-B84A-A571D54BD6BD}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{DF004809-5699-394D-AAFF-FFB449B25D85}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{C10AB038-D5E4-D340-9BF3-B8F1D5812D3D}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{96541ACC-E437-DD45-9983-F9CCE046975E}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{CEE06E54-8E14-F240-ABAB-95F7AD027D98}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{53783AA6-3689-AE46-A5D8-0425EDB0A4BC}"/>
+    <hyperlink ref="F29" r:id="rId28" xr:uid="{18C3BCD6-58FC-F541-8825-B978A5A2602C}"/>
+    <hyperlink ref="F30" r:id="rId29" xr:uid="{4D25F2A6-A490-3242-8979-DBEB2BF1A167}"/>
+    <hyperlink ref="F31" r:id="rId30" xr:uid="{5C392C48-8526-604F-AADC-E62FD00880F2}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{785AEEF5-4EB9-E04F-A1CD-51775C1B00B6}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{DE2E1597-3947-6345-9CA2-67ABDED98385}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{1878BA5C-673C-9B47-B7F5-9FBDF2085456}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>